<commit_message>
Continued development of parser...
</commit_message>
<xml_diff>
--- a/Jeopardy/Test.xlsx
+++ b/Jeopardy/Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75ADFA8-1FE7-433D-B781-B1684C004A35}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9704ADE-06D0-4223-BA72-9DCA4412CB65}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Valdkond-&gt;</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t xml:space="preserve">Täpselt nii palju vene tšikke on samal ajal majutatud Trummis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB! Don't change first 2 rows. </t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,14 +460,17 @@
     <col min="3" max="3" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -475,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>100</v>
       </c>
@@ -486,7 +492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>200</v>
       </c>
@@ -497,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>300</v>
       </c>
@@ -508,7 +514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>400</v>
       </c>
@@ -519,7 +525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>500</v>
       </c>
@@ -530,12 +536,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -546,14 +552,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>100</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>200</v>
       </c>
@@ -564,33 +570,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>300</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>400</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>500</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added very initial picture question implementation. Needs more work to be operational.
</commit_message>
<xml_diff>
--- a/Jeopardy/Test.xlsx
+++ b/Jeopardy/Test.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9704ADE-06D0-4223-BA72-9DCA4412CB65}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1753D4-5DF3-4DD4-9A9D-A193BEBFC16E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" calcMode="manual"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Valdkond-&gt;</t>
   </si>
@@ -91,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">NB! Don't change first 2 rows. </t>
+  </si>
+  <si>
+    <t>Pilt</t>
+  </si>
+  <si>
+    <t>example.jpg</t>
   </si>
 </sst>
 </file>
@@ -129,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -152,11 +153,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -166,6 +178,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,7 +465,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +495,9 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -523,6 +541,9 @@
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>